<commit_message>
small changes on dataset
</commit_message>
<xml_diff>
--- a/0_PrepDataSim/20240926_SelSimData.xlsx
+++ b/0_PrepDataSim/20240926_SelSimData.xlsx
@@ -477,10 +477,10 @@
         </is>
       </c>
       <c r="F2">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G2">
-        <v>74.40000000000001</v>
+        <v>75.8</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -542,10 +542,10 @@
         </is>
       </c>
       <c r="F3">
-        <v>1.81</v>
+        <v>169</v>
       </c>
       <c r="G3">
-        <v>104.6</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -607,10 +607,10 @@
         </is>
       </c>
       <c r="F4">
-        <v>1.68</v>
+        <v>165</v>
       </c>
       <c r="G4">
-        <v>73.90000000000001</v>
+        <v>71.7</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="F5">
-        <v>1.65</v>
+        <v>164</v>
       </c>
       <c r="G5">
         <v>68.40000000000001</v>
@@ -737,10 +737,10 @@
         </is>
       </c>
       <c r="F6">
-        <v>1.47</v>
+        <v>160</v>
       </c>
       <c r="G6">
-        <v>50.9</v>
+        <v>60.2</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -802,10 +802,10 @@
         </is>
       </c>
       <c r="F7">
-        <v>1.56</v>
+        <v>162</v>
       </c>
       <c r="G7">
-        <v>58.7</v>
+        <v>63.6</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -867,10 +867,10 @@
         </is>
       </c>
       <c r="F8">
-        <v>1.72</v>
+        <v>166</v>
       </c>
       <c r="G8">
-        <v>88.5</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="H8">
         <v>4</v>
@@ -932,10 +932,10 @@
         </is>
       </c>
       <c r="F9">
-        <v>1.61</v>
+        <v>163</v>
       </c>
       <c r="G9">
-        <v>72.59999999999999</v>
+        <v>75.2</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -997,10 +997,10 @@
         </is>
       </c>
       <c r="F10">
-        <v>1.69</v>
+        <v>166</v>
       </c>
       <c r="G10">
-        <v>74.8</v>
+        <v>72</v>
       </c>
       <c r="H10">
         <v>2</v>
@@ -1062,10 +1062,10 @@
         </is>
       </c>
       <c r="F11">
-        <v>1.69</v>
+        <v>166</v>
       </c>
       <c r="G11">
-        <v>69.90000000000001</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -1127,10 +1127,10 @@
         </is>
       </c>
       <c r="F12">
-        <v>1.68</v>
+        <v>165</v>
       </c>
       <c r="G12">
-        <v>84</v>
+        <v>81.5</v>
       </c>
       <c r="H12">
         <v>2</v>
@@ -1192,10 +1192,10 @@
         </is>
       </c>
       <c r="F13">
-        <v>1.57</v>
+        <v>162</v>
       </c>
       <c r="G13">
-        <v>80.3</v>
+        <v>86</v>
       </c>
       <c r="H13">
         <v>3</v>
@@ -1257,10 +1257,10 @@
         </is>
       </c>
       <c r="F14">
-        <v>1.74</v>
+        <v>167</v>
       </c>
       <c r="G14">
-        <v>76.8</v>
+        <v>70.90000000000001</v>
       </c>
       <c r="H14">
         <v>4</v>
@@ -1322,10 +1322,10 @@
         </is>
       </c>
       <c r="F15">
-        <v>1.56</v>
+        <v>162</v>
       </c>
       <c r="G15">
-        <v>51</v>
+        <v>55.5</v>
       </c>
       <c r="H15">
         <v>4</v>
@@ -1387,10 +1387,10 @@
         </is>
       </c>
       <c r="F16">
-        <v>1.65</v>
+        <v>165</v>
       </c>
       <c r="G16">
-        <v>63.5</v>
+        <v>63.2</v>
       </c>
       <c r="H16">
         <v>5</v>
@@ -1452,10 +1452,10 @@
         </is>
       </c>
       <c r="F17">
-        <v>1.54</v>
+        <v>161</v>
       </c>
       <c r="G17">
-        <v>59.6</v>
+        <v>66</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -1517,10 +1517,10 @@
         </is>
       </c>
       <c r="F18">
-        <v>1.56</v>
+        <v>162</v>
       </c>
       <c r="G18">
-        <v>59.5</v>
+        <v>64.3</v>
       </c>
       <c r="H18">
         <v>3</v>
@@ -1582,10 +1582,10 @@
         </is>
       </c>
       <c r="F19">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G19">
-        <v>81.59999999999999</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="H19">
         <v>4</v>
@@ -1647,10 +1647,10 @@
         </is>
       </c>
       <c r="F20">
-        <v>1.64</v>
+        <v>164</v>
       </c>
       <c r="G20">
-        <v>58.3</v>
+        <v>58.8</v>
       </c>
       <c r="H20">
         <v>4</v>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="F21">
-        <v>1.64</v>
+        <v>164</v>
       </c>
       <c r="G21">
-        <v>75.5</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="H21">
         <v>3</v>
@@ -1777,10 +1777,10 @@
         </is>
       </c>
       <c r="F22">
-        <v>1.67</v>
+        <v>165</v>
       </c>
       <c r="G22">
-        <v>72.5</v>
+        <v>71.3</v>
       </c>
       <c r="H22">
         <v>3</v>
@@ -1842,10 +1842,10 @@
         </is>
       </c>
       <c r="F23">
-        <v>1.67</v>
+        <v>165</v>
       </c>
       <c r="G23">
-        <v>73.90000000000001</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="H23">
         <v>4</v>
@@ -1907,10 +1907,10 @@
         </is>
       </c>
       <c r="F24">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G24">
-        <v>65.5</v>
+        <v>61.1</v>
       </c>
       <c r="H24">
         <v>5</v>
@@ -1972,10 +1972,10 @@
         </is>
       </c>
       <c r="F25">
-        <v>1.58</v>
+        <v>162</v>
       </c>
       <c r="G25">
-        <v>68.2</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="H25">
         <v>3</v>
@@ -2037,10 +2037,10 @@
         </is>
       </c>
       <c r="F26">
-        <v>1.67</v>
+        <v>165</v>
       </c>
       <c r="G26">
-        <v>74.2</v>
+        <v>72.7</v>
       </c>
       <c r="H26">
         <v>2</v>
@@ -2102,10 +2102,10 @@
         </is>
       </c>
       <c r="F27">
-        <v>1.57</v>
+        <v>162</v>
       </c>
       <c r="G27">
-        <v>69.40000000000001</v>
+        <v>74.8</v>
       </c>
       <c r="H27">
         <v>4</v>
@@ -2167,10 +2167,10 @@
         </is>
       </c>
       <c r="F28">
-        <v>1.46</v>
+        <v>159</v>
       </c>
       <c r="G28">
-        <v>52</v>
+        <v>62.4</v>
       </c>
       <c r="H28">
         <v>5</v>
@@ -2232,10 +2232,10 @@
         </is>
       </c>
       <c r="F29">
-        <v>1.51</v>
+        <v>161</v>
       </c>
       <c r="G29">
-        <v>61</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="H29">
         <v>5</v>
@@ -2297,10 +2297,10 @@
         </is>
       </c>
       <c r="F30">
-        <v>1.76</v>
+        <v>168</v>
       </c>
       <c r="G30">
-        <v>66.2</v>
+        <v>60.5</v>
       </c>
       <c r="H30">
         <v>5</v>
@@ -2362,10 +2362,10 @@
         </is>
       </c>
       <c r="F31">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G31">
-        <v>71</v>
+        <v>66.2</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -2427,10 +2427,10 @@
         </is>
       </c>
       <c r="F32">
-        <v>1.55</v>
+        <v>162</v>
       </c>
       <c r="G32">
-        <v>62.2</v>
+        <v>68.3</v>
       </c>
       <c r="H32">
         <v>3</v>
@@ -2492,10 +2492,10 @@
         </is>
       </c>
       <c r="F33">
-        <v>1.56</v>
+        <v>162</v>
       </c>
       <c r="G33">
-        <v>69.40000000000001</v>
+        <v>75.2</v>
       </c>
       <c r="H33">
         <v>3</v>
@@ -2557,10 +2557,10 @@
         </is>
       </c>
       <c r="F34">
-        <v>1.44</v>
+        <v>159</v>
       </c>
       <c r="G34">
-        <v>53.1</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="H34">
         <v>5</v>
@@ -2622,10 +2622,10 @@
         </is>
       </c>
       <c r="F35">
-        <v>1.58</v>
+        <v>162</v>
       </c>
       <c r="G35">
-        <v>52.5</v>
+        <v>56</v>
       </c>
       <c r="H35">
         <v>5</v>
@@ -2687,10 +2687,10 @@
         </is>
       </c>
       <c r="F36">
-        <v>1.76</v>
+        <v>168</v>
       </c>
       <c r="G36">
-        <v>84.90000000000001</v>
+        <v>77.5</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -2752,10 +2752,10 @@
         </is>
       </c>
       <c r="F37">
-        <v>1.58</v>
+        <v>163</v>
       </c>
       <c r="G37">
-        <v>61</v>
+        <v>64.8</v>
       </c>
       <c r="H37">
         <v>5</v>
@@ -2817,10 +2817,10 @@
         </is>
       </c>
       <c r="F38">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G38">
-        <v>75.09999999999999</v>
+        <v>70.09999999999999</v>
       </c>
       <c r="H38">
         <v>5</v>
@@ -2882,10 +2882,10 @@
         </is>
       </c>
       <c r="F39">
-        <v>1.58</v>
+        <v>162</v>
       </c>
       <c r="G39">
-        <v>64.3</v>
+        <v>68.7</v>
       </c>
       <c r="H39">
         <v>4</v>
@@ -2947,10 +2947,10 @@
         </is>
       </c>
       <c r="F40">
-        <v>1.65</v>
+        <v>165</v>
       </c>
       <c r="G40">
-        <v>74.09999999999999</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="H40">
         <v>3</v>
@@ -3012,10 +3012,10 @@
         </is>
       </c>
       <c r="F41">
-        <v>1.65</v>
+        <v>165</v>
       </c>
       <c r="G41">
-        <v>83.09999999999999</v>
+        <v>82.90000000000001</v>
       </c>
       <c r="H41">
         <v>5</v>
@@ -3077,10 +3077,10 @@
         </is>
       </c>
       <c r="F42">
-        <v>1.77</v>
+        <v>168</v>
       </c>
       <c r="G42">
-        <v>85.8</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="H42">
         <v>2</v>
@@ -3142,10 +3142,10 @@
         </is>
       </c>
       <c r="F43">
-        <v>1.82</v>
+        <v>169</v>
       </c>
       <c r="G43">
-        <v>79.59999999999999</v>
+        <v>69.2</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -3207,10 +3207,10 @@
         </is>
       </c>
       <c r="F44">
-        <v>1.6</v>
+        <v>163</v>
       </c>
       <c r="G44">
-        <v>62.3</v>
+        <v>65</v>
       </c>
       <c r="H44">
         <v>4</v>
@@ -3272,10 +3272,10 @@
         </is>
       </c>
       <c r="F45">
-        <v>1.57</v>
+        <v>162</v>
       </c>
       <c r="G45">
-        <v>62.9</v>
+        <v>67.5</v>
       </c>
       <c r="H45">
         <v>3</v>
@@ -3337,10 +3337,10 @@
         </is>
       </c>
       <c r="F46">
-        <v>1.79</v>
+        <v>168</v>
       </c>
       <c r="G46">
-        <v>78.5</v>
+        <v>70.09999999999999</v>
       </c>
       <c r="H46">
         <v>2</v>
@@ -3402,10 +3402,10 @@
         </is>
       </c>
       <c r="F47">
-        <v>1.58</v>
+        <v>163</v>
       </c>
       <c r="G47">
-        <v>67.59999999999999</v>
+        <v>71.7</v>
       </c>
       <c r="H47">
         <v>3</v>
@@ -3467,10 +3467,10 @@
         </is>
       </c>
       <c r="F48">
-        <v>1.7</v>
+        <v>166</v>
       </c>
       <c r="G48">
-        <v>70.59999999999999</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="H48">
         <v>4</v>
@@ -3532,10 +3532,10 @@
         </is>
       </c>
       <c r="F49">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G49">
-        <v>70.59999999999999</v>
+        <v>72</v>
       </c>
       <c r="H49">
         <v>5</v>
@@ -3597,10 +3597,10 @@
         </is>
       </c>
       <c r="F50">
-        <v>1.69</v>
+        <v>166</v>
       </c>
       <c r="G50">
-        <v>80.40000000000001</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="H50">
         <v>5</v>
@@ -3662,10 +3662,10 @@
         </is>
       </c>
       <c r="F51">
-        <v>1.59</v>
+        <v>163</v>
       </c>
       <c r="G51">
-        <v>59.7</v>
+        <v>63.1</v>
       </c>
       <c r="H51">
         <v>4</v>
@@ -3727,10 +3727,10 @@
         </is>
       </c>
       <c r="F52">
-        <v>1.79</v>
+        <v>168</v>
       </c>
       <c r="G52">
-        <v>92.09999999999999</v>
+        <v>81.90000000000001</v>
       </c>
       <c r="H52">
         <v>4</v>
@@ -3792,10 +3792,10 @@
         </is>
       </c>
       <c r="F53">
-        <v>1.58</v>
+        <v>163</v>
       </c>
       <c r="G53">
-        <v>72.8</v>
+        <v>77.3</v>
       </c>
       <c r="H53">
         <v>4</v>
@@ -3857,10 +3857,10 @@
         </is>
       </c>
       <c r="F54">
-        <v>1.76</v>
+        <v>167</v>
       </c>
       <c r="G54">
-        <v>90.2</v>
+        <v>82.5</v>
       </c>
       <c r="H54">
         <v>2</v>
@@ -3922,10 +3922,10 @@
         </is>
       </c>
       <c r="F55">
-        <v>1.77</v>
+        <v>168</v>
       </c>
       <c r="G55">
-        <v>81.09999999999999</v>
+        <v>73.3</v>
       </c>
       <c r="H55">
         <v>3</v>
@@ -3987,10 +3987,10 @@
         </is>
       </c>
       <c r="F56">
-        <v>1.75</v>
+        <v>167</v>
       </c>
       <c r="G56">
-        <v>91.3</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="H56">
         <v>2</v>
@@ -4052,10 +4052,10 @@
         </is>
       </c>
       <c r="F57">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G57">
-        <v>80.3</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="H57">
         <v>3</v>
@@ -4117,10 +4117,10 @@
         </is>
       </c>
       <c r="F58">
-        <v>1.59</v>
+        <v>163</v>
       </c>
       <c r="G58">
-        <v>79</v>
+        <v>83.7</v>
       </c>
       <c r="H58">
         <v>5</v>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="F59">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G59">
-        <v>97.8</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="H59">
         <v>3</v>
@@ -4247,10 +4247,10 @@
         </is>
       </c>
       <c r="F60">
-        <v>1.8</v>
+        <v>169</v>
       </c>
       <c r="G60">
-        <v>84.2</v>
+        <v>74.3</v>
       </c>
       <c r="H60">
         <v>5</v>
@@ -4312,10 +4312,10 @@
         </is>
       </c>
       <c r="F61">
-        <v>1.61</v>
+        <v>163</v>
       </c>
       <c r="G61">
-        <v>58.4</v>
+        <v>60.4</v>
       </c>
       <c r="H61">
         <v>3</v>
@@ -4377,10 +4377,10 @@
         </is>
       </c>
       <c r="F62">
-        <v>1.45</v>
+        <v>159</v>
       </c>
       <c r="G62">
-        <v>61.3</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="H62">
         <v>3</v>
@@ -4442,10 +4442,10 @@
         </is>
       </c>
       <c r="F63">
-        <v>1.8</v>
+        <v>169</v>
       </c>
       <c r="G63">
-        <v>76.90000000000001</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="H63">
         <v>2</v>
@@ -4507,10 +4507,10 @@
         </is>
       </c>
       <c r="F64">
-        <v>1.81</v>
+        <v>169</v>
       </c>
       <c r="G64">
-        <v>70.59999999999999</v>
+        <v>61.9</v>
       </c>
       <c r="H64">
         <v>5</v>
@@ -4572,10 +4572,10 @@
         </is>
       </c>
       <c r="F65">
-        <v>1.53</v>
+        <v>161</v>
       </c>
       <c r="G65">
-        <v>62.1</v>
+        <v>69.3</v>
       </c>
       <c r="H65">
         <v>3</v>
@@ -4637,10 +4637,10 @@
         </is>
       </c>
       <c r="F66">
-        <v>1.43</v>
+        <v>158</v>
       </c>
       <c r="G66">
-        <v>51.3</v>
+        <v>63.5</v>
       </c>
       <c r="H66">
         <v>2</v>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="F67">
-        <v>1.7</v>
+        <v>166</v>
       </c>
       <c r="G67">
-        <v>81.59999999999999</v>
+        <v>78.5</v>
       </c>
       <c r="H67">
         <v>3</v>
@@ -4767,10 +4767,10 @@
         </is>
       </c>
       <c r="F68">
-        <v>1.59</v>
+        <v>163</v>
       </c>
       <c r="G68">
-        <v>72.3</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="H68">
         <v>2</v>
@@ -4832,10 +4832,10 @@
         </is>
       </c>
       <c r="F69">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G69">
-        <v>67.40000000000001</v>
+        <v>68.7</v>
       </c>
       <c r="H69">
         <v>5</v>
@@ -4897,10 +4897,10 @@
         </is>
       </c>
       <c r="F70">
-        <v>1.64</v>
+        <v>164</v>
       </c>
       <c r="G70">
-        <v>68</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="H70">
         <v>3</v>
@@ -4962,10 +4962,10 @@
         </is>
       </c>
       <c r="F71">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G71">
-        <v>83.90000000000001</v>
+        <v>78.7</v>
       </c>
       <c r="H71">
         <v>4</v>
@@ -5027,10 +5027,10 @@
         </is>
       </c>
       <c r="F72">
-        <v>1.79</v>
+        <v>168</v>
       </c>
       <c r="G72">
-        <v>73.90000000000001</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="H72">
         <v>3</v>
@@ -5092,10 +5092,10 @@
         </is>
       </c>
       <c r="F73">
-        <v>1.72</v>
+        <v>166</v>
       </c>
       <c r="G73">
-        <v>78</v>
+        <v>73.8</v>
       </c>
       <c r="H73">
         <v>5</v>
@@ -5157,10 +5157,10 @@
         </is>
       </c>
       <c r="F74">
-        <v>1.72</v>
+        <v>167</v>
       </c>
       <c r="G74">
-        <v>79.90000000000001</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="H74">
         <v>2</v>
@@ -5222,10 +5222,10 @@
         </is>
       </c>
       <c r="F75">
-        <v>1.79</v>
+        <v>169</v>
       </c>
       <c r="G75">
-        <v>69</v>
+        <v>61.3</v>
       </c>
       <c r="H75">
         <v>3</v>
@@ -5287,10 +5287,10 @@
         </is>
       </c>
       <c r="F76">
-        <v>1.55</v>
+        <v>162</v>
       </c>
       <c r="G76">
-        <v>65.09999999999999</v>
+        <v>71.2</v>
       </c>
       <c r="H76">
         <v>2</v>
@@ -5352,10 +5352,10 @@
         </is>
       </c>
       <c r="F77">
-        <v>1.65</v>
+        <v>165</v>
       </c>
       <c r="G77">
-        <v>63.2</v>
+        <v>63</v>
       </c>
       <c r="H77">
         <v>4</v>
@@ -5417,10 +5417,10 @@
         </is>
       </c>
       <c r="F78">
-        <v>1.62</v>
+        <v>164</v>
       </c>
       <c r="G78">
-        <v>68.90000000000001</v>
+        <v>70.8</v>
       </c>
       <c r="H78">
         <v>4</v>
@@ -5482,10 +5482,10 @@
         </is>
       </c>
       <c r="F79">
-        <v>1.68</v>
+        <v>165</v>
       </c>
       <c r="G79">
-        <v>76.8</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="H79">
         <v>5</v>
@@ -5547,10 +5547,10 @@
         </is>
       </c>
       <c r="F80">
-        <v>1.75</v>
+        <v>167</v>
       </c>
       <c r="G80">
-        <v>85.59999999999999</v>
+        <v>78.5</v>
       </c>
       <c r="H80">
         <v>5</v>
@@ -5612,10 +5612,10 @@
         </is>
       </c>
       <c r="F81">
-        <v>1.68</v>
+        <v>165</v>
       </c>
       <c r="G81">
-        <v>65.8</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="H81">
         <v>2</v>
@@ -5677,10 +5677,10 @@
         </is>
       </c>
       <c r="F82">
-        <v>1.58</v>
+        <v>163</v>
       </c>
       <c r="G82">
-        <v>64.3</v>
+        <v>68.3</v>
       </c>
       <c r="H82">
         <v>5</v>
@@ -5742,10 +5742,10 @@
         </is>
       </c>
       <c r="F83">
-        <v>1.75</v>
+        <v>167</v>
       </c>
       <c r="G83">
-        <v>85.3</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="H83">
         <v>3</v>
@@ -5807,10 +5807,10 @@
         </is>
       </c>
       <c r="F84">
-        <v>1.77</v>
+        <v>168</v>
       </c>
       <c r="G84">
-        <v>92.2</v>
+        <v>83.5</v>
       </c>
       <c r="H84">
         <v>2</v>
@@ -5872,10 +5872,10 @@
         </is>
       </c>
       <c r="F85">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G85">
-        <v>67.59999999999999</v>
+        <v>68.5</v>
       </c>
       <c r="H85">
         <v>4</v>
@@ -5937,10 +5937,10 @@
         </is>
       </c>
       <c r="F86">
-        <v>1.56</v>
+        <v>162</v>
       </c>
       <c r="G86">
-        <v>67</v>
+        <v>72.7</v>
       </c>
       <c r="H86">
         <v>5</v>
@@ -6002,10 +6002,10 @@
         </is>
       </c>
       <c r="F87">
-        <v>1.57</v>
+        <v>162</v>
       </c>
       <c r="G87">
-        <v>69.59999999999999</v>
+        <v>74.8</v>
       </c>
       <c r="H87">
         <v>3</v>
@@ -6067,10 +6067,10 @@
         </is>
       </c>
       <c r="F88">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G88">
-        <v>65.5</v>
+        <v>66.8</v>
       </c>
       <c r="H88">
         <v>3</v>
@@ -6132,7 +6132,7 @@
         </is>
       </c>
       <c r="F89">
-        <v>1.65</v>
+        <v>164</v>
       </c>
       <c r="G89">
         <v>69.59999999999999</v>
@@ -6197,10 +6197,10 @@
         </is>
       </c>
       <c r="F90">
-        <v>1.67</v>
+        <v>165</v>
       </c>
       <c r="G90">
-        <v>75.5</v>
+        <v>74.3</v>
       </c>
       <c r="H90">
         <v>2</v>
@@ -6262,10 +6262,10 @@
         </is>
       </c>
       <c r="F91">
-        <v>1.59</v>
+        <v>163</v>
       </c>
       <c r="G91">
-        <v>60.8</v>
+        <v>64.2</v>
       </c>
       <c r="H91">
         <v>2</v>
@@ -6327,10 +6327,10 @@
         </is>
       </c>
       <c r="F92">
-        <v>1.68</v>
+        <v>165</v>
       </c>
       <c r="G92">
-        <v>71.2</v>
+        <v>69.3</v>
       </c>
       <c r="H92">
         <v>2</v>
@@ -6392,10 +6392,10 @@
         </is>
       </c>
       <c r="F93">
-        <v>1.77</v>
+        <v>168</v>
       </c>
       <c r="G93">
-        <v>66.2</v>
+        <v>59.8</v>
       </c>
       <c r="H93">
         <v>4</v>
@@ -6457,10 +6457,10 @@
         </is>
       </c>
       <c r="F94">
-        <v>1.57</v>
+        <v>162</v>
       </c>
       <c r="G94">
-        <v>65.5</v>
+        <v>70.09999999999999</v>
       </c>
       <c r="H94">
         <v>3</v>
@@ -6522,10 +6522,10 @@
         </is>
       </c>
       <c r="F95">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G95">
-        <v>73</v>
+        <v>68.2</v>
       </c>
       <c r="H95">
         <v>3</v>
@@ -6587,10 +6587,10 @@
         </is>
       </c>
       <c r="F96">
-        <v>1.66</v>
+        <v>165</v>
       </c>
       <c r="G96">
-        <v>65.2</v>
+        <v>64.5</v>
       </c>
       <c r="H96">
         <v>3</v>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="F97">
-        <v>1.75</v>
+        <v>167</v>
       </c>
       <c r="G97">
-        <v>84.8</v>
+        <v>77.8</v>
       </c>
       <c r="H97">
         <v>4</v>
@@ -6717,10 +6717,10 @@
         </is>
       </c>
       <c r="F98">
-        <v>1.66</v>
+        <v>165</v>
       </c>
       <c r="G98">
-        <v>74.8</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="H98">
         <v>3</v>
@@ -6782,10 +6782,10 @@
         </is>
       </c>
       <c r="F99">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G99">
-        <v>91.5</v>
+        <v>85.3</v>
       </c>
       <c r="H99">
         <v>4</v>
@@ -6847,10 +6847,10 @@
         </is>
       </c>
       <c r="F100">
-        <v>1.67</v>
+        <v>165</v>
       </c>
       <c r="G100">
-        <v>72</v>
+        <v>70.7</v>
       </c>
       <c r="H100">
         <v>5</v>
@@ -6912,10 +6912,10 @@
         </is>
       </c>
       <c r="F101">
-        <v>1.8</v>
+        <v>169</v>
       </c>
       <c r="G101">
-        <v>91.2</v>
+        <v>80.8</v>
       </c>
       <c r="H101">
         <v>5</v>
@@ -6977,10 +6977,10 @@
         </is>
       </c>
       <c r="F102">
-        <v>1.58</v>
+        <v>163</v>
       </c>
       <c r="G102">
-        <v>66.3</v>
+        <v>70.7</v>
       </c>
       <c r="H102">
         <v>2</v>
@@ -7042,10 +7042,10 @@
         </is>
       </c>
       <c r="F103">
-        <v>1.67</v>
+        <v>165</v>
       </c>
       <c r="G103">
-        <v>68.3</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="H103">
         <v>5</v>
@@ -7107,10 +7107,10 @@
         </is>
       </c>
       <c r="F104">
-        <v>1.55</v>
+        <v>162</v>
       </c>
       <c r="G104">
-        <v>65.3</v>
+        <v>71.8</v>
       </c>
       <c r="H104">
         <v>2</v>
@@ -7172,10 +7172,10 @@
         </is>
       </c>
       <c r="F105">
-        <v>1.7</v>
+        <v>166</v>
       </c>
       <c r="G105">
-        <v>77.2</v>
+        <v>74</v>
       </c>
       <c r="H105">
         <v>2</v>
@@ -7237,10 +7237,10 @@
         </is>
       </c>
       <c r="F106">
-        <v>1.56</v>
+        <v>162</v>
       </c>
       <c r="G106">
-        <v>56.9</v>
+        <v>61.9</v>
       </c>
       <c r="H106">
         <v>3</v>
@@ -7302,10 +7302,10 @@
         </is>
       </c>
       <c r="F107">
-        <v>1.61</v>
+        <v>163</v>
       </c>
       <c r="G107">
-        <v>64.3</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="H107">
         <v>2</v>
@@ -7367,10 +7367,10 @@
         </is>
       </c>
       <c r="F108">
-        <v>1.55</v>
+        <v>162</v>
       </c>
       <c r="G108">
-        <v>62.3</v>
+        <v>68.3</v>
       </c>
       <c r="H108">
         <v>2</v>
@@ -7432,10 +7432,10 @@
         </is>
       </c>
       <c r="F109">
-        <v>1.6</v>
+        <v>163</v>
       </c>
       <c r="G109">
-        <v>66.7</v>
+        <v>69.5</v>
       </c>
       <c r="H109">
         <v>2</v>
@@ -7497,10 +7497,10 @@
         </is>
       </c>
       <c r="F110">
-        <v>1.64</v>
+        <v>164</v>
       </c>
       <c r="G110">
-        <v>62.3</v>
+        <v>62.9</v>
       </c>
       <c r="H110">
         <v>5</v>
@@ -7562,10 +7562,10 @@
         </is>
       </c>
       <c r="F111">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G111">
-        <v>59.3</v>
+        <v>60.3</v>
       </c>
       <c r="H111">
         <v>4</v>
@@ -7627,10 +7627,10 @@
         </is>
       </c>
       <c r="F112">
-        <v>1.48</v>
+        <v>160</v>
       </c>
       <c r="G112">
-        <v>56.6</v>
+        <v>66.5</v>
       </c>
       <c r="H112">
         <v>3</v>
@@ -7692,10 +7692,10 @@
         </is>
       </c>
       <c r="F113">
-        <v>1.69</v>
+        <v>166</v>
       </c>
       <c r="G113">
-        <v>71.3</v>
+        <v>69</v>
       </c>
       <c r="H113">
         <v>2</v>
@@ -7757,10 +7757,10 @@
         </is>
       </c>
       <c r="F114">
-        <v>1.76</v>
+        <v>168</v>
       </c>
       <c r="G114">
-        <v>77.2</v>
+        <v>70.3</v>
       </c>
       <c r="H114">
         <v>5</v>
@@ -7822,10 +7822,10 @@
         </is>
       </c>
       <c r="F115">
-        <v>1.75</v>
+        <v>167</v>
       </c>
       <c r="G115">
-        <v>89.7</v>
+        <v>82.40000000000001</v>
       </c>
       <c r="H115">
         <v>2</v>
@@ -7887,10 +7887,10 @@
         </is>
       </c>
       <c r="F116">
-        <v>1.62</v>
+        <v>164</v>
       </c>
       <c r="G116">
-        <v>62.5</v>
+        <v>63.9</v>
       </c>
       <c r="H116">
         <v>2</v>
@@ -7952,10 +7952,10 @@
         </is>
       </c>
       <c r="F117">
-        <v>1.79</v>
+        <v>169</v>
       </c>
       <c r="G117">
-        <v>71.09999999999999</v>
+        <v>63.2</v>
       </c>
       <c r="H117">
         <v>3</v>
@@ -8017,10 +8017,10 @@
         </is>
       </c>
       <c r="F118">
-        <v>1.59</v>
+        <v>163</v>
       </c>
       <c r="G118">
-        <v>59.4</v>
+        <v>62.6</v>
       </c>
       <c r="H118">
         <v>3</v>
@@ -8082,10 +8082,10 @@
         </is>
       </c>
       <c r="F119">
-        <v>1.68</v>
+        <v>165</v>
       </c>
       <c r="G119">
-        <v>71</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="H119">
         <v>2</v>
@@ -8147,10 +8147,10 @@
         </is>
       </c>
       <c r="F120">
-        <v>1.52</v>
+        <v>161</v>
       </c>
       <c r="G120">
-        <v>59.5</v>
+        <v>67.2</v>
       </c>
       <c r="H120">
         <v>5</v>
@@ -8212,10 +8212,10 @@
         </is>
       </c>
       <c r="F121">
-        <v>1.75</v>
+        <v>167</v>
       </c>
       <c r="G121">
-        <v>67</v>
+        <v>61.5</v>
       </c>
       <c r="H121">
         <v>2</v>
@@ -8277,10 +8277,10 @@
         </is>
       </c>
       <c r="F122">
-        <v>1.57</v>
+        <v>162</v>
       </c>
       <c r="G122">
-        <v>64.09999999999999</v>
+        <v>69</v>
       </c>
       <c r="H122">
         <v>5</v>
@@ -8342,10 +8342,10 @@
         </is>
       </c>
       <c r="F123">
-        <v>1.62</v>
+        <v>164</v>
       </c>
       <c r="G123">
-        <v>59.9</v>
+        <v>61.5</v>
       </c>
       <c r="H123">
         <v>3</v>
@@ -8407,10 +8407,10 @@
         </is>
       </c>
       <c r="F124">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G124">
-        <v>85.5</v>
+        <v>87.2</v>
       </c>
       <c r="H124">
         <v>2</v>
@@ -8472,10 +8472,10 @@
         </is>
       </c>
       <c r="F125">
-        <v>1.57</v>
+        <v>162</v>
       </c>
       <c r="G125">
-        <v>56.1</v>
+        <v>60.4</v>
       </c>
       <c r="H125">
         <v>2</v>
@@ -8537,10 +8537,10 @@
         </is>
       </c>
       <c r="F126">
-        <v>1.68</v>
+        <v>165</v>
       </c>
       <c r="G126">
-        <v>67.90000000000001</v>
+        <v>66</v>
       </c>
       <c r="H126">
         <v>5</v>
@@ -8602,10 +8602,10 @@
         </is>
       </c>
       <c r="F127">
-        <v>1.74</v>
+        <v>167</v>
       </c>
       <c r="G127">
-        <v>74.09999999999999</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="H127">
         <v>2</v>
@@ -8667,10 +8667,10 @@
         </is>
       </c>
       <c r="F128">
-        <v>1.7</v>
+        <v>166</v>
       </c>
       <c r="G128">
-        <v>63.6</v>
+        <v>60.7</v>
       </c>
       <c r="H128">
         <v>2</v>
@@ -8732,10 +8732,10 @@
         </is>
       </c>
       <c r="F129">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G129">
-        <v>70.8</v>
+        <v>72.2</v>
       </c>
       <c r="H129">
         <v>4</v>
@@ -8797,10 +8797,10 @@
         </is>
       </c>
       <c r="F130">
-        <v>1.71</v>
+        <v>166</v>
       </c>
       <c r="G130">
-        <v>74.90000000000001</v>
+        <v>71.3</v>
       </c>
       <c r="H130">
         <v>4</v>
@@ -8862,10 +8862,10 @@
         </is>
       </c>
       <c r="F131">
-        <v>1.57</v>
+        <v>162</v>
       </c>
       <c r="G131">
-        <v>70.8</v>
+        <v>76.3</v>
       </c>
       <c r="H131">
         <v>5</v>
@@ -8927,10 +8927,10 @@
         </is>
       </c>
       <c r="F132">
-        <v>1.66</v>
+        <v>165</v>
       </c>
       <c r="G132">
-        <v>79.09999999999999</v>
+        <v>78.2</v>
       </c>
       <c r="H132">
         <v>2</v>
@@ -8992,10 +8992,10 @@
         </is>
       </c>
       <c r="F133">
-        <v>1.79</v>
+        <v>168</v>
       </c>
       <c r="G133">
-        <v>77.2</v>
+        <v>69</v>
       </c>
       <c r="H133">
         <v>4</v>
@@ -9057,10 +9057,10 @@
         </is>
       </c>
       <c r="F134">
-        <v>1.71</v>
+        <v>166</v>
       </c>
       <c r="G134">
-        <v>77.3</v>
+        <v>73.5</v>
       </c>
       <c r="H134">
         <v>5</v>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="F135">
-        <v>1.68</v>
+        <v>165</v>
       </c>
       <c r="G135">
-        <v>78.09999999999999</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="H135">
         <v>4</v>
@@ -9187,10 +9187,10 @@
         </is>
       </c>
       <c r="F136">
-        <v>1.68</v>
+        <v>165</v>
       </c>
       <c r="G136">
-        <v>80.3</v>
+        <v>78.3</v>
       </c>
       <c r="H136">
         <v>5</v>
@@ -9252,10 +9252,10 @@
         </is>
       </c>
       <c r="F137">
-        <v>1.66</v>
+        <v>165</v>
       </c>
       <c r="G137">
-        <v>66.09999999999999</v>
+        <v>65.3</v>
       </c>
       <c r="H137">
         <v>4</v>
@@ -9317,10 +9317,10 @@
         </is>
       </c>
       <c r="F138">
-        <v>1.86</v>
+        <v>171</v>
       </c>
       <c r="G138">
-        <v>91.59999999999999</v>
+        <v>77.09999999999999</v>
       </c>
       <c r="H138">
         <v>4</v>
@@ -9382,10 +9382,10 @@
         </is>
       </c>
       <c r="F139">
-        <v>1.64</v>
+        <v>164</v>
       </c>
       <c r="G139">
-        <v>69.40000000000001</v>
+        <v>69.7</v>
       </c>
       <c r="H139">
         <v>5</v>
@@ -9447,10 +9447,10 @@
         </is>
       </c>
       <c r="F140">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G140">
-        <v>73.40000000000001</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="H140">
         <v>5</v>
@@ -9512,10 +9512,10 @@
         </is>
       </c>
       <c r="F141">
-        <v>1.55</v>
+        <v>162</v>
       </c>
       <c r="G141">
-        <v>59.2</v>
+        <v>64.5</v>
       </c>
       <c r="H141">
         <v>3</v>
@@ -9577,10 +9577,10 @@
         </is>
       </c>
       <c r="F142">
-        <v>1.56</v>
+        <v>162</v>
       </c>
       <c r="G142">
-        <v>72.7</v>
+        <v>78.7</v>
       </c>
       <c r="H142">
         <v>5</v>
@@ -9642,10 +9642,10 @@
         </is>
       </c>
       <c r="F143">
-        <v>1.54</v>
+        <v>161</v>
       </c>
       <c r="G143">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H143">
         <v>3</v>
@@ -9707,10 +9707,10 @@
         </is>
       </c>
       <c r="F144">
-        <v>1.75</v>
+        <v>167</v>
       </c>
       <c r="G144">
-        <v>79.8</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="H144">
         <v>3</v>
@@ -9772,10 +9772,10 @@
         </is>
       </c>
       <c r="F145">
-        <v>1.51</v>
+        <v>160</v>
       </c>
       <c r="G145">
-        <v>50.3</v>
+        <v>57.5</v>
       </c>
       <c r="H145">
         <v>4</v>
@@ -9837,10 +9837,10 @@
         </is>
       </c>
       <c r="F146">
-        <v>1.57</v>
+        <v>162</v>
       </c>
       <c r="G146">
-        <v>51.9</v>
+        <v>55.7</v>
       </c>
       <c r="H146">
         <v>2</v>
@@ -9902,10 +9902,10 @@
         </is>
       </c>
       <c r="F147">
-        <v>1.75</v>
+        <v>167</v>
       </c>
       <c r="G147">
-        <v>86.09999999999999</v>
+        <v>79.3</v>
       </c>
       <c r="H147">
         <v>5</v>
@@ -9967,10 +9967,10 @@
         </is>
       </c>
       <c r="F148">
-        <v>1.62</v>
+        <v>164</v>
       </c>
       <c r="G148">
-        <v>63</v>
+        <v>64.8</v>
       </c>
       <c r="H148">
         <v>4</v>
@@ -10032,10 +10032,10 @@
         </is>
       </c>
       <c r="F149">
-        <v>1.69</v>
+        <v>166</v>
       </c>
       <c r="G149">
-        <v>67.59999999999999</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="H149">
         <v>3</v>
@@ -10097,10 +10097,10 @@
         </is>
       </c>
       <c r="F150">
-        <v>1.64</v>
+        <v>164</v>
       </c>
       <c r="G150">
-        <v>67.3</v>
+        <v>67.7</v>
       </c>
       <c r="H150">
         <v>5</v>
@@ -10162,10 +10162,10 @@
         </is>
       </c>
       <c r="F151">
-        <v>1.71</v>
+        <v>166</v>
       </c>
       <c r="G151">
-        <v>80.2</v>
+        <v>76.2</v>
       </c>
       <c r="H151">
         <v>4</v>
@@ -10227,10 +10227,10 @@
         </is>
       </c>
       <c r="F152">
-        <v>1.54</v>
+        <v>162</v>
       </c>
       <c r="G152">
-        <v>62.1</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="H152">
         <v>3</v>
@@ -10292,10 +10292,10 @@
         </is>
       </c>
       <c r="F153">
-        <v>1.6</v>
+        <v>163</v>
       </c>
       <c r="G153">
-        <v>67.40000000000001</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="H153">
         <v>4</v>
@@ -10357,10 +10357,10 @@
         </is>
       </c>
       <c r="F154">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G154">
-        <v>78.40000000000001</v>
+        <v>79.90000000000001</v>
       </c>
       <c r="H154">
         <v>3</v>
@@ -10422,10 +10422,10 @@
         </is>
       </c>
       <c r="F155">
-        <v>1.52</v>
+        <v>161</v>
       </c>
       <c r="G155">
-        <v>56.8</v>
+        <v>63.9</v>
       </c>
       <c r="H155">
         <v>3</v>
@@ -10487,10 +10487,10 @@
         </is>
       </c>
       <c r="F156">
-        <v>1.72</v>
+        <v>167</v>
       </c>
       <c r="G156">
-        <v>66.59999999999999</v>
+        <v>62.6</v>
       </c>
       <c r="H156">
         <v>4</v>
@@ -10552,10 +10552,10 @@
         </is>
       </c>
       <c r="F157">
-        <v>1.63</v>
+        <v>164</v>
       </c>
       <c r="G157">
-        <v>81</v>
+        <v>82.8</v>
       </c>
       <c r="H157">
         <v>3</v>
@@ -10617,10 +10617,10 @@
         </is>
       </c>
       <c r="F158">
-        <v>1.73</v>
+        <v>167</v>
       </c>
       <c r="G158">
-        <v>84.09999999999999</v>
+        <v>78.5</v>
       </c>
       <c r="H158">
         <v>2</v>
@@ -10682,10 +10682,10 @@
         </is>
       </c>
       <c r="F159">
-        <v>1.6</v>
+        <v>163</v>
       </c>
       <c r="G159">
-        <v>75.59999999999999</v>
+        <v>79</v>
       </c>
       <c r="H159">
         <v>3</v>

</xml_diff>